<commit_message>
slight changes to schema
</commit_message>
<xml_diff>
--- a/mini project/Schema.xlsx
+++ b/mini project/Schema.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>users</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>responses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id </t>
   </si>
   <si>
     <t>fullname</t>
@@ -101,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -113,6 +110,11 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
       <sz val="12.0"/>
@@ -183,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -192,11 +194,14 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -430,22 +435,22 @@
       <c r="D3" s="2"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" ht="18.0" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="C5" s="5"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1">
@@ -467,17 +472,17 @@
       <c r="O7" s="2"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" ht="21.75" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="3"/>
@@ -521,40 +526,40 @@
       <c r="M11" s="2"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" ht="24.0" customHeight="1">
       <c r="B12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="3"/>
+      <c r="J12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="N12" s="3"/>
     </row>
@@ -562,7 +567,7 @@
     <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -570,21 +575,21 @@
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" ht="18.75" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -1574,18 +1579,18 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="B11:N11"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B15:G15"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B15:G15"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:P7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
     <mergeCell ref="O8:P8"/>
   </mergeCells>
   <printOptions/>

</xml_diff>